<commit_message>
added all experiment data
</commit_message>
<xml_diff>
--- a/experiment/Score.xlsx
+++ b/experiment/Score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BasicData" sheetId="3" r:id="rId1"/>
@@ -129,7 +129,7 @@
     <t>Location Prediction Accuracy</t>
   </si>
   <si>
-    <t>Tap96</t>
+    <t>IphoneData</t>
   </si>
 </sst>
 </file>
@@ -322,13 +322,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>155.7863847407693</c:v>
+                  <c:v>0.329097579933149</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>229.0408591018719</c:v>
+                  <c:v>0.474599523238272</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.08789821083216</c:v>
+                  <c:v>0.155572695604305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -382,13 +382,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>582.1072584868951</c:v>
+                  <c:v>0.392357190464239</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1039.380243096875</c:v>
+                  <c:v>0.41784116022106</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.49220376822113</c:v>
+                  <c:v>0.104906188346589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -442,13 +442,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>401.0139011385685</c:v>
+                  <c:v>0.295557133196011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1023.997666177457</c:v>
+                  <c:v>0.485825847480232</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>25.49220376822113</c:v>
+                  <c:v>0.104906188346589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -464,11 +464,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2109986448"/>
-        <c:axId val="-2082882208"/>
+        <c:axId val="-2079068624"/>
+        <c:axId val="-2079065216"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2109986448"/>
+        <c:axId val="-2079068624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2082882208"/>
+        <c:crossAx val="-2079065216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -518,7 +518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2082882208"/>
+        <c:axId val="-2079065216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -538,6 +538,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -568,7 +569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2109986448"/>
+        <c:crossAx val="-2079068624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -779,13 +780,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.148148148148148</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.555555555555556</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.111111111111111</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -839,10 +840,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.222222222222222</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.185185185185185</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.111111111111111</c:v>
@@ -899,10 +900,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0.444444444444444</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.407407407407407</c:v>
+                  <c:v>0.111111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.111111111111111</c:v>
@@ -921,11 +922,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2062163888"/>
-        <c:axId val="-2062160560"/>
+        <c:axId val="-2079040368"/>
+        <c:axId val="-2079037040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2062163888"/>
+        <c:axId val="-2079040368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,7 +968,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062160560"/>
+        <c:crossAx val="-2079037040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -975,7 +976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2062160560"/>
+        <c:axId val="-2079037040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1026,7 +1027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062163888"/>
+        <c:crossAx val="-2079040368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1263,7 +1264,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -1281,7 +1282,7 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -1385,13 +1386,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -1483,10 +1484,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.0</c:v>
@@ -1495,13 +1496,13 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -1521,11 +1522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062116080"/>
-        <c:axId val="-2062113024"/>
+        <c:axId val="-2107141104"/>
+        <c:axId val="-2107138048"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2062116080"/>
+        <c:axId val="-2107141104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1567,7 +1568,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062113024"/>
+        <c:crossAx val="-2107138048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1575,7 +1576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2062113024"/>
+        <c:axId val="-2107138048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1625,7 +1626,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062116080"/>
+        <c:crossAx val="-2107141104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1862,31 +1863,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.666666666666667</c:v>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.666666666666667</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.666666666666667</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1975,22 +1976,22 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.666666666666667</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -2085,16 +2086,16 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.666666666666667</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.0</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0.0</c:v>
@@ -2120,11 +2121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062070128"/>
-        <c:axId val="-2062067072"/>
+        <c:axId val="-2107697984"/>
+        <c:axId val="-2107694928"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2062070128"/>
+        <c:axId val="-2107697984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2166,7 +2167,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062067072"/>
+        <c:crossAx val="-2107694928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2174,7 +2175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2062067072"/>
+        <c:axId val="-2107694928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2225,7 +2226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062070128"/>
+        <c:crossAx val="-2107697984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2462,7 +2463,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.0</c:v>
@@ -2480,7 +2481,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -2720,11 +2721,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2062024544"/>
-        <c:axId val="-2062021488"/>
+        <c:axId val="-2079855808"/>
+        <c:axId val="-2079852752"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2062024544"/>
+        <c:axId val="-2079855808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,7 +2767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062021488"/>
+        <c:crossAx val="-2079852752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2774,7 +2775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2062021488"/>
+        <c:axId val="-2079852752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2824,7 +2825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2062024544"/>
+        <c:crossAx val="-2079855808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2838,6 +2839,344 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Prediction</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Accuracy</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Summery!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>cross-correlation</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Summery!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>linear</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>diagonal</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>diwl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Summery!$D$5:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.111111111111111</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2061730208"/>
+        <c:axId val="-2031038080"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2061730208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2031038080"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2031038080"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2061730208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3072,6 +3411,43 @@
   <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -5626,6 +6002,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5773,6 +6652,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495301</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -6182,8 +7093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="H15" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6245,39 +7156,39 @@
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="H2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!H$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="I2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!I$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="J2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!J$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="K2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!K$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="L2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!L$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="M2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!M$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="N2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!N$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="O2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!O$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="P2">
         <f ca="1">COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!P$1)</f>
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.2">
@@ -6305,15 +7216,15 @@
       </c>
       <c r="B5">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A5, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A5, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$4)</f>
-        <v>0.14814814814814814</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C5">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A5, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A5, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$4)</f>
-        <v>0</v>
+        <v>0.22222222222222221</v>
       </c>
       <c r="D5">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A5, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A5, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$4)</f>
-        <v>0</v>
+        <v>0.44444444444444442</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -6322,15 +7233,15 @@
       </c>
       <c r="B6">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A6, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A6, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$4)</f>
-        <v>0.55555555555555558</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C6">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A6, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A6, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$4)</f>
-        <v>0.18518518518518517</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D6">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A6, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A6, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$4)</f>
-        <v>0.40740740740740738</v>
+        <v>0.1111111111111111</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
@@ -6339,7 +7250,7 @@
       </c>
       <c r="B7">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A7, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A7, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$4)</f>
-        <v>0.1111111111111111</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="C7">
         <f ca="1">COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A7, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$4, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A7, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$4)</f>
@@ -6374,16 +7285,16 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A12, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$11)</f>
-        <v>155.78638474076934</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A12, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$11) / SUM($H$2:$P$2)</f>
+        <v>0.32909757993314859</v>
       </c>
       <c r="C12">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A12, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$11)</f>
-        <v>582.10725848689515</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A12, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$11) / SUM($H$2:$P$2)</f>
+        <v>0.39235719046423917</v>
       </c>
       <c r="D12">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A12, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$11)</f>
-        <v>401.01390113856849</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A12, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$11) / SUM($H$2:$P$2)</f>
+        <v>0.29555713319601101</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
@@ -6391,16 +7302,16 @@
         <v>6</v>
       </c>
       <c r="B13">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A13, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$11)</f>
-        <v>229.04085910187186</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A13, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$11) / SUM($H$2:$P$2)</f>
+        <v>0.47459952323827193</v>
       </c>
       <c r="C13">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A13, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$11)</f>
-        <v>1039.3802430968753</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A13, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$11) / SUM($H$2:$P$2)</f>
+        <v>0.41784116022105972</v>
       </c>
       <c r="D13">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A13, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$11)</f>
-        <v>1023.9976661774572</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A13, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$11) / SUM($H$2:$P$2)</f>
+        <v>0.4858258474802325</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
@@ -6408,16 +7319,16 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A14, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$11)</f>
-        <v>26.087898210832158</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A14, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$11) / SUM($H$2:$P$2)</f>
+        <v>0.15557269560430501</v>
       </c>
       <c r="C14">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A14, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$11)</f>
-        <v>25.492203768221135</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A14, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$11) / SUM($H$2:$P$2)</f>
+        <v>0.10490618834658896</v>
       </c>
       <c r="D14">
-        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A14, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$11)</f>
-        <v>25.492203768221135</v>
+        <f ca="1">SUMIFS(INDIRECT(CONCATENATE($B$1, "!$H:$H")), INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A14, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$11) / SUM($H$2:$P$2)</f>
+        <v>0.10490618834658896</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -6445,7 +7356,7 @@
       </c>
       <c r="B21">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21), 0)</f>
@@ -6453,7 +7364,7 @@
       </c>
       <c r="D21">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A21), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -6470,7 +7381,7 @@
       </c>
       <c r="D22">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A22) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A22, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A22), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -6517,11 +7428,11 @@
       </c>
       <c r="C25">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A25) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A25, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A25), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A25) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A25, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A25), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -6547,15 +7458,15 @@
       </c>
       <c r="B27">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27), 0)</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="C27">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$20, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$20, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A27), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -6612,7 +7523,7 @@
       </c>
       <c r="B33">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A33) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A33, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A33), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A33) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A33, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A33), 0)</f>
@@ -6629,15 +7540,15 @@
       </c>
       <c r="B34">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34), 0)</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="C34">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34), 0)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="D34">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A34), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -6646,15 +7557,15 @@
       </c>
       <c r="B35">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C35">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35), 0)</f>
-        <v>0.33333333333333331</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A35), 0)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -6663,7 +7574,7 @@
       </c>
       <c r="B36">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C36">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36), 0)</f>
@@ -6671,7 +7582,7 @@
       </c>
       <c r="D36">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A36), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -6680,15 +7591,15 @@
       </c>
       <c r="B37">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37), 0)</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="C37">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37), 0)</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A37), 0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -6697,7 +7608,7 @@
       </c>
       <c r="B38">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A38) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A38, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A38), 0)</f>
-        <v>0.66666666666666663</v>
+        <v>1</v>
       </c>
       <c r="C38">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A38) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A38, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A38), 0)</f>
@@ -6714,11 +7625,11 @@
       </c>
       <c r="B39">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C39">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D39">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!D$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A39), 0)</f>
@@ -6731,7 +7642,7 @@
       </c>
       <c r="B40">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A40) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A40, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A40), 0)</f>
-        <v>0.66666666666666663</v>
+        <v>0</v>
       </c>
       <c r="C40">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A40) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A40, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A40), 0)</f>
@@ -6748,7 +7659,7 @@
       </c>
       <c r="B41">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A41) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A41, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A41), 0)</f>
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="C41">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A41) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A41, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$32, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$32, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A41), 0)</f>
@@ -6779,7 +7690,7 @@
       </c>
       <c r="B45">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A45) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A45, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A45), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C45">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A45) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A45, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A45), 0)</f>
@@ -6881,7 +7792,7 @@
       </c>
       <c r="B51">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A51) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A51, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!B$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A51), 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C51">
         <f ca="1">IF(COUNTIF(INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A51) &gt; 0, COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A51, INDIRECT(CONCATENATE($B$1, "!$I:$I")), TRUE) / COUNTIFS(INDIRECT(CONCATENATE($B$1, "!$A:$A")), Summery!$A$44, INDIRECT(CONCATENATE($B$1, "!$B:$B")), Summery!C$44, INDIRECT(CONCATENATE($B$1, "!$F:$F")), Summery!$A51), 0)</f>

</xml_diff>

<commit_message>
updated documentation of the final result
</commit_message>
<xml_diff>
--- a/experiment/Score.xlsx
+++ b/experiment/Score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16040" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BasicData" sheetId="3" r:id="rId1"/>
@@ -464,11 +464,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2079068624"/>
-        <c:axId val="-2079065216"/>
+        <c:axId val="-2096301568"/>
+        <c:axId val="-2096298160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079068624"/>
+        <c:axId val="-2096301568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +510,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079065216"/>
+        <c:crossAx val="-2096298160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -518,7 +518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079065216"/>
+        <c:axId val="-2096298160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -569,7 +569,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079068624"/>
+        <c:crossAx val="-2096301568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -922,11 +922,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2079040368"/>
-        <c:axId val="-2079037040"/>
+        <c:axId val="-2094395808"/>
+        <c:axId val="-2094392480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2079040368"/>
+        <c:axId val="-2094395808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -968,7 +968,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079037040"/>
+        <c:crossAx val="-2094392480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -976,7 +976,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079037040"/>
+        <c:axId val="-2094392480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -1027,7 +1027,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079040368"/>
+        <c:crossAx val="-2094395808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1522,11 +1522,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2107141104"/>
-        <c:axId val="-2107138048"/>
+        <c:axId val="-2114436688"/>
+        <c:axId val="-2114433632"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2107141104"/>
+        <c:axId val="-2114436688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1568,7 +1568,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107138048"/>
+        <c:crossAx val="-2114433632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1576,7 +1576,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107138048"/>
+        <c:axId val="-2114433632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1626,7 +1626,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107141104"/>
+        <c:crossAx val="-2114436688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2121,11 +2121,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2107697984"/>
-        <c:axId val="-2107694928"/>
+        <c:axId val="-2094321376"/>
+        <c:axId val="-2094318320"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2107697984"/>
+        <c:axId val="-2094321376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,7 +2167,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107694928"/>
+        <c:crossAx val="-2094318320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2175,7 +2175,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2107694928"/>
+        <c:axId val="-2094318320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2226,7 +2226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2107697984"/>
+        <c:crossAx val="-2094321376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2721,11 +2721,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079855808"/>
-        <c:axId val="-2079852752"/>
+        <c:axId val="-2094275728"/>
+        <c:axId val="-2094272672"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-2079855808"/>
+        <c:axId val="-2094275728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2767,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079852752"/>
+        <c:crossAx val="-2094272672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2775,7 +2775,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2079852752"/>
+        <c:axId val="-2094272672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2825,7 +2825,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079855808"/>
+        <c:crossAx val="-2094275728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3058,11 +3058,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2061730208"/>
-        <c:axId val="-2031038080"/>
+        <c:axId val="-2094246288"/>
+        <c:axId val="-2094243024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061730208"/>
+        <c:axId val="-2094246288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3104,7 +3104,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2031038080"/>
+        <c:crossAx val="-2094243024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3112,7 +3112,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2031038080"/>
+        <c:axId val="-2094243024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.0"/>
@@ -3163,7 +3163,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061730208"/>
+        <c:crossAx val="-2094246288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7093,7 +7093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H15" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>

</xml_diff>